<commit_message>
initialised object repository for website + tested initialise state
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1E3FD-92EA-4453-A751-E7E6393E9D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -51,47 +51,13 @@
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
     <t>LogMessage_Success</t>
   </si>
   <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>LogMessage_BusinessRuleException</t>
-  </si>
-  <si>
-    <t>Business rule exception.</t>
-  </si>
-  <si>
     <t>LogMessage_ApplicationException</t>
   </si>
   <si>
-    <t>System exception.</t>
-  </si>
-  <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -112,15 +78,9 @@
     <t>Static part of logging message. Processed Transaction succesful.</t>
   </si>
   <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
     <t>Static part of logging message. Processed Transaction failed with application exception.</t>
   </si>
   <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
@@ -130,18 +90,6 @@
     <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
   </si>
   <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
     <t>OrchestratorQueueFolder</t>
   </si>
   <si>
@@ -161,13 +109,43 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools_Queue</t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools</t>
+  </si>
+  <si>
+    <t>https://www.privateschoolreview.com/</t>
+  </si>
+  <si>
+    <t>PrivateSchoolReviewHomeUrl</t>
+  </si>
+  <si>
+    <t>Url to main page of privateschoolreview.com site containing list of states</t>
+  </si>
+  <si>
+    <t>LogMessage_Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items not added to queue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items Successfully added to queue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System exception. </t>
+  </si>
+  <si>
+    <t>ListUSAPrivateSchools_Dispatcher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -191,6 +169,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,26 +208,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -591,50 +590,67 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{13B3E025-D591-44CF-8D81-D44E7EEC9AC8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -684,27 +700,25 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
@@ -721,104 +735,52 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
+      <c r="B7" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+      <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
-      <c r="A12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="A14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="5" t="b">
+    <row r="12" spans="1:26" ht="30.75" customHeight="1">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +813,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
added logic to retrieve state data row from dt (get next transaction)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1E3FD-92EA-4453-A751-E7E6393E9D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B423FD2-CC08-4F3D-8EC3-CB16534F5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -126,19 +126,52 @@
     <t>Url to main page of privateschoolreview.com site containing list of states</t>
   </si>
   <si>
-    <t>LogMessage_Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Items not added to queue. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Items Successfully added to queue. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System exception. </t>
-  </si>
-  <si>
     <t>ListUSAPrivateSchools_Dispatcher</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
 </sst>
 </file>
@@ -542,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -618,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>
@@ -647,10 +680,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -733,53 +766,100 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>34</v>
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="30.75" customHeight="1">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="b">
+      <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added creating report at the beginning of the process and setting asset to be used in producer process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\ListUSAPrivateSchools\ListUSAPrivateSchools_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B423FD2-CC08-4F3D-8EC3-CB16534F5F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEEC2A1-BECA-4C48-8306-5EF11812DB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ReportTemplateFilepath</t>
+  </si>
+  <si>
+    <t>Data\ReportTemplate.xlsx</t>
+  </si>
+  <si>
+    <t>path to file which contains template for output report</t>
+  </si>
+  <si>
+    <t>ReportFilepathPattern</t>
+  </si>
+  <si>
+    <t>CurrentReportFilepath</t>
+  </si>
+  <si>
+    <t>D:\UiPath Projects\ListUSAPrivateSchools\Reports\USAPrivateSchools_&lt;replace_timestamp&gt;.xlsx</t>
+  </si>
+  <si>
+    <t>CurrentReportFilepathAssetName</t>
+  </si>
+  <si>
+    <t>Asset to store filepath to report created by dispatcher - will be utilised by one or many producers to populate the single report</t>
+  </si>
+  <si>
+    <t>Name of the orchestrator folder which contains Asset to store current report filepath</t>
   </si>
 </sst>
 </file>
@@ -573,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -668,6 +695,50 @@
         <v>32</v>
       </c>
     </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -682,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -871,10 +942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1919,7 +1990,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>